<commit_message>
water budget edited and lulc added
</commit_message>
<xml_diff>
--- a/iJal/app/static/assets/water_budget.xlsx
+++ b/iJal/app/static/assets/water_budget.xlsx
@@ -103,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -121,11 +121,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -496,7 +499,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M56"/>
+  <dimension ref="A1:M60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,19 +507,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="51" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="34" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="2" max="2"/>
     <col width="6" customWidth="1" min="3" max="3"/>
     <col width="6" customWidth="1" min="4" max="4"/>
     <col width="36" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="6" customWidth="1" min="9" max="9"/>
     <col width="26" customWidth="1" min="10" max="10"/>
-    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="22" customWidth="1" min="11" max="11"/>
     <col width="18" customWidth="1" min="12" max="12"/>
-    <col width="11" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -571,7 +574,7 @@
       </c>
       <c r="B5" s="5" t="inlineStr">
         <is>
-          <t>Andhra Pradesh</t>
+          <t>Uttar Pradesh</t>
         </is>
       </c>
       <c r="E5" s="6" t="inlineStr">
@@ -593,7 +596,7 @@
       </c>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Alluri Sitharama Raju</t>
+          <t>Aligarh</t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
@@ -635,7 +638,7 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>Gangavaram</t>
+          <t>Gangiri</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
@@ -644,10 +647,10 @@
         </is>
       </c>
       <c r="F7" s="8" t="n">
-        <v>12393</v>
+        <v>143696</v>
       </c>
       <c r="G7" s="8" t="n">
-        <v>31.1</v>
+        <v>360.59</v>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
@@ -655,10 +658,10 @@
         </is>
       </c>
       <c r="K7" s="8" t="n">
-        <v>12</v>
+        <v>140</v>
       </c>
       <c r="L7" s="8" t="n">
-        <v>1.51</v>
+        <v>10.95</v>
       </c>
     </row>
     <row r="8">
@@ -668,7 +671,7 @@
         </is>
       </c>
       <c r="B8" s="5" t="n">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
@@ -676,10 +679,10 @@
         </is>
       </c>
       <c r="F8" s="8" t="n">
-        <v>13519</v>
+        <v>126279</v>
       </c>
       <c r="G8" s="8" t="n">
-        <v>33.92</v>
+        <v>316.88</v>
       </c>
       <c r="J8" s="5" t="inlineStr">
         <is>
@@ -687,10 +690,10 @@
         </is>
       </c>
       <c r="K8" s="8" t="n">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="L8" s="8" t="n">
-        <v>47.59</v>
+        <v>46.89</v>
       </c>
     </row>
     <row r="9">
@@ -700,36 +703,42 @@
         </is>
       </c>
       <c r="B9" s="5" t="n">
-        <v>75728.31</v>
+        <v>52924.36</v>
+      </c>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>269975</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <v>677.47</v>
       </c>
       <c r="J9" s="5" t="inlineStr">
         <is>
-          <t>Resevoirs</t>
+          <t>Lakes</t>
         </is>
       </c>
       <c r="K9" s="8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L9" s="8" t="n">
-        <v>162</v>
+        <v>49.43</v>
       </c>
     </row>
     <row r="10">
-      <c r="E10" s="6" t="inlineStr">
-        <is>
-          <t>b) Livestock(in HaM)</t>
-        </is>
-      </c>
       <c r="J10" s="5" t="inlineStr">
         <is>
-          <t>Others</t>
+          <t>Ponds</t>
         </is>
       </c>
       <c r="K10" s="8" t="n">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="L10" s="8" t="n">
-        <v>770.75</v>
+        <v>103.21</v>
       </c>
     </row>
     <row r="11">
@@ -738,44 +747,49 @@
           <t>WATER TRANSFER</t>
         </is>
       </c>
-      <c r="E11" s="7" t="inlineStr">
+      <c r="E11" s="6" t="inlineStr">
+        <is>
+          <t>b) Livestock(in HaM)</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>Resevoirs</t>
+        </is>
+      </c>
+      <c r="K11" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" s="8" t="n">
+        <v>225.06</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="E12" s="7" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="F11" s="7" t="inlineStr">
+      <c r="F12" s="7" t="inlineStr">
         <is>
           <t>Count</t>
         </is>
       </c>
-      <c r="G11" s="7" t="inlineStr">
+      <c r="G12" s="7" t="inlineStr">
         <is>
           <t>Consumption</t>
         </is>
       </c>
-      <c r="J11" s="5" t="inlineStr">
-        <is>
-          <t>Ponds</t>
-        </is>
-      </c>
-      <c r="K11" s="8" t="n">
-        <v>600</v>
-      </c>
-      <c r="L11" s="8" t="n">
-        <v>805.6</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="E12" s="5" t="inlineStr">
-        <is>
-          <t>Cattle</t>
-        </is>
-      </c>
-      <c r="F12" s="8" t="n">
-        <v>8329</v>
-      </c>
-      <c r="G12" s="8" t="n">
-        <v>20.37</v>
+      <c r="J12" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="K12" s="10" t="n">
+        <v>330</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>435.54</v>
       </c>
     </row>
     <row r="13">
@@ -791,19 +805,14 @@
       </c>
       <c r="E13" s="5" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Cattle</t>
         </is>
       </c>
       <c r="F13" s="8" t="n">
-        <v>1627</v>
+        <v>21899</v>
       </c>
       <c r="G13" s="8" t="n">
-        <v>3.98</v>
-      </c>
-      <c r="J13" s="6" t="inlineStr">
-        <is>
-          <t>b) Groundwater(in HaM)</t>
-        </is>
+        <v>53.55</v>
       </c>
     </row>
     <row r="14">
@@ -812,28 +821,23 @@
           <t>Inward (Drinking)</t>
         </is>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B14" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="5" t="inlineStr">
         <is>
-          <t>Sheep</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="F14" s="8" t="n">
-        <v>1977</v>
+        <v>111287</v>
       </c>
       <c r="G14" s="8" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="J14" s="7" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="K14" s="7" t="inlineStr">
-        <is>
-          <t>Value</t>
+        <v>272.15</v>
+      </c>
+      <c r="J14" s="6" t="inlineStr">
+        <is>
+          <t>b) Groundwater(in HaM)</t>
         </is>
       </c>
     </row>
@@ -843,27 +847,29 @@
           <t>Inward (Industry)</t>
         </is>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="5" t="inlineStr">
         <is>
-          <t>Goat</t>
+          <t>Sheep</t>
         </is>
       </c>
       <c r="F15" s="8" t="n">
-        <v>6274</v>
+        <v>176</v>
       </c>
       <c r="G15" s="8" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="J15" s="5" t="inlineStr">
-        <is>
-          <t>Extractable Groundwater</t>
-        </is>
-      </c>
-      <c r="K15" s="8" t="n">
-        <v>4367.82</v>
+        <v>0.04</v>
+      </c>
+      <c r="J15" s="7" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="K15" s="7" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -872,27 +878,27 @@
           <t>Inward (Irrigation)</t>
         </is>
       </c>
-      <c r="B16" s="9" t="n">
-        <v>57092.43</v>
+      <c r="B16" s="11" t="n">
+        <v>0.2</v>
       </c>
       <c r="E16" s="5" t="inlineStr">
         <is>
-          <t>Pig</t>
+          <t>Goat</t>
         </is>
       </c>
       <c r="F16" s="8" t="n">
-        <v>28</v>
+        <v>17318</v>
       </c>
       <c r="G16" s="8" t="n">
-        <v>0.02</v>
+        <v>4.42</v>
       </c>
       <c r="J16" s="5" t="inlineStr">
         <is>
-          <t>Extracted Groundwater</t>
+          <t>Extractable Groundwater</t>
         </is>
       </c>
       <c r="K16" s="8" t="n">
-        <v>46.35</v>
+        <v>7859.98</v>
       </c>
     </row>
     <row r="17">
@@ -901,27 +907,27 @@
           <t>Outward (Drinking)</t>
         </is>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="11" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="5" t="inlineStr">
         <is>
-          <t>Poultry</t>
+          <t>Pig</t>
         </is>
       </c>
       <c r="F17" s="8" t="n">
-        <v>18995</v>
+        <v>180</v>
       </c>
       <c r="G17" s="8" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.14</v>
       </c>
       <c r="J17" s="5" t="inlineStr">
         <is>
-          <t>Stage of Extraction</t>
+          <t>Extracted Groundwater</t>
         </is>
       </c>
       <c r="K17" s="8" t="n">
-        <v>1.08</v>
+        <v>6847.99</v>
       </c>
     </row>
     <row r="18">
@@ -930,18 +936,27 @@
           <t>Outward (Industry)</t>
         </is>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="11" t="n">
         <v>0</v>
       </c>
+      <c r="E18" s="5" t="inlineStr">
+        <is>
+          <t>Poultry</t>
+        </is>
+      </c>
+      <c r="F18" s="8" t="n">
+        <v>250</v>
+      </c>
+      <c r="G18" s="8" t="n">
+        <v>0.01</v>
+      </c>
       <c r="J18" s="5" t="inlineStr">
         <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="K18" s="5" t="inlineStr">
-        <is>
-          <t>safe</t>
-        </is>
+          <t>Stage of Extraction</t>
+        </is>
+      </c>
+      <c r="K18" s="8" t="n">
+        <v>87.12</v>
       </c>
     </row>
     <row r="19">
@@ -950,680 +965,1038 @@
           <t>Outward (Irrigation)</t>
         </is>
       </c>
-      <c r="B19" s="9" t="n">
+      <c r="B19" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="6" t="inlineStr">
+      <c r="E19" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="F19" s="10" t="n">
+        <v>151110</v>
+      </c>
+      <c r="G19" s="10" t="n">
+        <v>330.31</v>
+      </c>
+      <c r="J19" s="5" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="K19" s="5" t="inlineStr">
+        <is>
+          <t>semi-critical</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B20" s="11" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" s="6" t="inlineStr">
         <is>
           <t>c) Crops(in HaM)</t>
         </is>
       </c>
-    </row>
-    <row r="20">
-      <c r="E20" s="7" t="inlineStr">
+      <c r="J21" s="6" t="inlineStr">
+        <is>
+          <t>c) Runoff(in HaM)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>WATER BUDGET</t>
+        </is>
+      </c>
+      <c r="E22" s="7" t="inlineStr">
         <is>
           <t>Crop</t>
         </is>
       </c>
-      <c r="F20" s="7" t="inlineStr">
+      <c r="F22" s="7" t="inlineStr">
         <is>
           <t>Area</t>
         </is>
       </c>
-      <c r="G20" s="7" t="inlineStr">
+      <c r="G22" s="7" t="inlineStr">
         <is>
           <t>Consumption</t>
         </is>
       </c>
-      <c r="J20" s="6" t="inlineStr">
-        <is>
-          <t>c) Runoff(in HaM)</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
-        <is>
-          <t>WATER BUDGET</t>
-        </is>
-      </c>
-      <c r="E21" s="5" t="inlineStr">
-        <is>
-          <t>Rice</t>
-        </is>
-      </c>
-      <c r="F21" s="8" t="n">
-        <v>1188</v>
-      </c>
-      <c r="G21" s="8" t="n">
-        <v>1782</v>
-      </c>
-      <c r="J21" s="7" t="inlineStr">
+      <c r="J22" s="7" t="inlineStr">
         <is>
           <t>Catchment</t>
         </is>
       </c>
-      <c r="K21" s="7" t="inlineStr">
+      <c r="K22" s="7" t="inlineStr">
         <is>
           <t>% Runoff</t>
         </is>
       </c>
-      <c r="L21" s="7" t="inlineStr">
+      <c r="L22" s="7" t="inlineStr">
         <is>
           <t>Yield</t>
         </is>
       </c>
-      <c r="M21" s="7" t="inlineStr">
+      <c r="M22" s="7" t="inlineStr">
         <is>
           <t>Available</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="E22" s="5" t="inlineStr">
-        <is>
-          <t>Cashewnut</t>
-        </is>
-      </c>
-      <c r="F22" s="8" t="n">
-        <v>2695</v>
-      </c>
-      <c r="G22" s="8" t="n">
-        <v>1347.5</v>
-      </c>
-      <c r="J22" s="5" t="inlineStr">
+    <row r="23">
+      <c r="E23" s="5" t="inlineStr">
+        <is>
+          <t>Wheat</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="n">
+        <v>16895</v>
+      </c>
+      <c r="G23" s="8" t="n">
+        <v>9292.25</v>
+      </c>
+      <c r="J23" s="5" t="inlineStr">
         <is>
           <t>Good Catchment</t>
         </is>
       </c>
-      <c r="K22" s="8" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="L22" s="8" t="n">
-        <v>3719.62</v>
-      </c>
-      <c r="M22" s="8" t="n">
-        <v>184277.53</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="7" t="inlineStr">
+      <c r="K23" s="8" t="n">
+        <v>38.6</v>
+      </c>
+      <c r="L23" s="8" t="n">
+        <v>3983.83</v>
+      </c>
+      <c r="M23" s="8" t="n">
+        <v>6145.95</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="7" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B23" s="7" t="inlineStr">
+      <c r="B24" s="7" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="E23" s="5" t="inlineStr">
-        <is>
-          <t>Tapioca</t>
-        </is>
-      </c>
-      <c r="F23" s="8" t="n">
-        <v>219</v>
-      </c>
-      <c r="G23" s="8" t="n">
-        <v>109.5</v>
-      </c>
-      <c r="J23" s="5" t="inlineStr">
+      <c r="E24" s="5" t="inlineStr">
+        <is>
+          <t>Mustard</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="n">
+        <v>7621</v>
+      </c>
+      <c r="G24" s="8" t="n">
+        <v>3810.5</v>
+      </c>
+      <c r="J24" s="5" t="inlineStr">
         <is>
           <t>Average Catchment</t>
         </is>
       </c>
-      <c r="K23" s="8" t="n">
-        <v>28.1</v>
-      </c>
-      <c r="L23" s="8" t="n">
-        <v>2787.24</v>
-      </c>
-      <c r="M23" s="8" t="n">
-        <v>4258.9</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="10" t="inlineStr">
+      <c r="K24" s="8" t="n">
+        <v>28.9</v>
+      </c>
+      <c r="L24" s="8" t="n">
+        <v>2982.71</v>
+      </c>
+      <c r="M24" s="8" t="n">
+        <v>422.48</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9" t="inlineStr">
         <is>
           <t>Demand</t>
         </is>
       </c>
-      <c r="B24" s="11" t="n"/>
-      <c r="E24" s="5" t="inlineStr">
-        <is>
-          <t>Mango</t>
-        </is>
-      </c>
-      <c r="F24" s="8" t="n">
-        <v>70</v>
-      </c>
-      <c r="G24" s="8" t="n">
-        <v>42</v>
-      </c>
-      <c r="J24" s="5" t="inlineStr">
+      <c r="B25" s="12" t="n"/>
+      <c r="E25" s="5" t="inlineStr">
+        <is>
+          <t>Bajra</t>
+        </is>
+      </c>
+      <c r="F25" s="8" t="n">
+        <v>7414</v>
+      </c>
+      <c r="G25" s="8" t="n">
+        <v>2965.6</v>
+      </c>
+      <c r="J25" s="5" t="inlineStr">
         <is>
           <t>Bad Catchment</t>
         </is>
       </c>
-      <c r="K24" s="8" t="n">
-        <v>18.7</v>
-      </c>
-      <c r="L24" s="8" t="n">
-        <v>1854.85</v>
-      </c>
-      <c r="M24" s="8" t="n">
-        <v>45737.41</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="inlineStr">
-        <is>
-          <t>Human Population Consumption</t>
-        </is>
-      </c>
-      <c r="B25" s="9" t="n">
-        <v>65.02</v>
-      </c>
-      <c r="E25" s="5" t="inlineStr">
-        <is>
-          <t>Cotton(lint)</t>
-        </is>
-      </c>
-      <c r="F25" s="8" t="n">
-        <v>39</v>
-      </c>
-      <c r="G25" s="8" t="n">
-        <v>33.15</v>
+      <c r="K25" s="8" t="n">
+        <v>19.3</v>
+      </c>
+      <c r="L25" s="8" t="n">
+        <v>1991.91</v>
+      </c>
+      <c r="M25" s="8" t="n">
+        <v>7186.95</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5" t="inlineStr">
         <is>
-          <t>Livestock Population Consumption</t>
-        </is>
-      </c>
-      <c r="B26" s="9" t="n">
-        <v>27.17</v>
+          <t>Human Population Consumption</t>
+        </is>
+      </c>
+      <c r="B26" s="11" t="n">
+        <v>677.47</v>
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>Other oilseeds</t>
+          <t>Banana</t>
         </is>
       </c>
       <c r="F26" s="8" t="n">
-        <v>48</v>
+        <v>1083.62</v>
       </c>
       <c r="G26" s="8" t="n">
-        <v>24</v>
-      </c>
-      <c r="J26" s="6" t="inlineStr">
-        <is>
-          <t>d) LULC(in HaM)</t>
-        </is>
+        <v>2383.96</v>
+      </c>
+      <c r="J26" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="K26" s="7" t="inlineStr"/>
+      <c r="L26" s="10" t="n">
+        <v>8958.450000000001</v>
+      </c>
+      <c r="M26" s="10" t="n">
+        <v>13755.38</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
-          <t>Crops Consumption</t>
-        </is>
-      </c>
-      <c r="B27" s="9" t="n">
-        <v>3340.55</v>
+          <t>Livestock Population Consumption</t>
+        </is>
+      </c>
+      <c r="B27" s="11" t="n">
+        <v>330.31</v>
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
-          <t>Ragi</t>
+          <t>Potato</t>
         </is>
       </c>
       <c r="F27" s="8" t="n">
-        <v>4</v>
+        <v>1900</v>
       </c>
       <c r="G27" s="8" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="J27" s="7" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="K27" s="7" t="inlineStr">
-        <is>
-          <t>Area</t>
-        </is>
+        <v>1140</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="5" t="inlineStr">
         <is>
+          <t>Crops Consumption</t>
+        </is>
+      </c>
+      <c r="B28" s="11" t="n">
+        <v>22073.65</v>
+      </c>
+      <c r="E28" s="5" t="inlineStr">
+        <is>
+          <t>Castor seed</t>
+        </is>
+      </c>
+      <c r="F28" s="8" t="n">
+        <v>1494.36</v>
+      </c>
+      <c r="G28" s="8" t="n">
+        <v>1046.05</v>
+      </c>
+      <c r="J28" s="6" t="inlineStr">
+        <is>
+          <t>d) LULC(in HaM)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="inlineStr">
+        <is>
           <t>Industry Consumption</t>
         </is>
       </c>
-      <c r="B28" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5" t="inlineStr">
-        <is>
-          <t>Maize</t>
-        </is>
-      </c>
-      <c r="F28" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="8" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="J28" s="5" t="inlineStr">
+      <c r="B29" s="11" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="E29" s="5" t="inlineStr">
+        <is>
+          <t>Arhar</t>
+        </is>
+      </c>
+      <c r="F29" s="8" t="n">
+        <v>1358.76</v>
+      </c>
+      <c r="G29" s="8" t="n">
+        <v>543.5</v>
+      </c>
+      <c r="J29" s="7" t="inlineStr">
+        <is>
+          <t>Catchment</t>
+        </is>
+      </c>
+      <c r="K29" s="7" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="L29" s="7" t="inlineStr">
+        <is>
+          <t>Area</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="9" t="inlineStr">
+        <is>
+          <t>Supply</t>
+        </is>
+      </c>
+      <c r="B30" s="12" t="n"/>
+      <c r="E30" s="5" t="inlineStr">
+        <is>
+          <t>Barley</t>
+        </is>
+      </c>
+      <c r="F30" s="8" t="n">
+        <v>505</v>
+      </c>
+      <c r="G30" s="8" t="n">
+        <v>277.75</v>
+      </c>
+      <c r="J30" s="5" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="K30" s="5" t="inlineStr">
         <is>
           <t>Forest Area</t>
         </is>
       </c>
-      <c r="K28" s="8" t="n">
-        <v>42532</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="10" t="inlineStr">
-        <is>
-          <t>Supply</t>
-        </is>
-      </c>
-      <c r="B29" s="11" t="n"/>
-      <c r="J29" s="5" t="inlineStr">
-        <is>
-          <t>Non Agriculture Area</t>
-        </is>
-      </c>
-      <c r="K29" s="8" t="n">
-        <v>2677.02</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="5" t="inlineStr">
-        <is>
-          <t>Available Surface Water</t>
-        </is>
-      </c>
-      <c r="B30" s="9" t="n">
-        <v>1787.45</v>
-      </c>
-      <c r="E30" s="6" t="inlineStr">
-        <is>
-          <t>d) Industry(in HaM)</t>
-        </is>
-      </c>
-      <c r="J30" s="5" t="inlineStr">
-        <is>
-          <t>Uncultivable Area</t>
-        </is>
-      </c>
-      <c r="K30" s="8" t="n">
-        <v>4333.01</v>
+      <c r="L30" s="8" t="n">
+        <v>13247.06</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="inlineStr">
         <is>
-          <t>Ground Water</t>
-        </is>
-      </c>
-      <c r="B31" s="9" t="n">
-        <v>46.35</v>
-      </c>
-      <c r="E31" s="7" t="inlineStr">
-        <is>
-          <t>*No industries in this block</t>
-        </is>
+          <t>Available Surface Water</t>
+        </is>
+      </c>
+      <c r="B31" s="11" t="n">
+        <v>435.54</v>
+      </c>
+      <c r="E31" s="5" t="inlineStr">
+        <is>
+          <t>Cotton(lint)</t>
+        </is>
+      </c>
+      <c r="F31" s="8" t="n">
+        <v>220</v>
+      </c>
+      <c r="G31" s="8" t="n">
+        <v>187</v>
       </c>
       <c r="J31" s="5" t="inlineStr">
         <is>
-          <t>Grazing Area</t>
-        </is>
-      </c>
-      <c r="K31" s="8" t="n">
-        <v>1081</v>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="K31" s="5" t="inlineStr">
+        <is>
+          <t>Non Agriculture Area</t>
+        </is>
+      </c>
+      <c r="L31" s="8" t="n">
+        <v>495.48</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="5" t="inlineStr">
         <is>
-          <t>Water Transfer Inward</t>
-        </is>
-      </c>
-      <c r="B32" s="9" t="n">
-        <v>57092.43</v>
+          <t>Ground Water</t>
+        </is>
+      </c>
+      <c r="B32" s="11" t="n">
+        <v>6847.99</v>
+      </c>
+      <c r="E32" s="5" t="inlineStr">
+        <is>
+          <t>Maize</t>
+        </is>
+      </c>
+      <c r="F32" s="8" t="n">
+        <v>231.95</v>
+      </c>
+      <c r="G32" s="8" t="n">
+        <v>139.17</v>
       </c>
       <c r="J32" s="5" t="inlineStr">
         <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="K32" s="5" t="inlineStr">
+        <is>
+          <t>Uncultivable Area</t>
+        </is>
+      </c>
+      <c r="L32" s="8" t="n">
+        <v>1684.7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>Water Transfer Outward</t>
+        </is>
+      </c>
+      <c r="B33" s="11" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E33" s="5" t="inlineStr">
+        <is>
+          <t>Tobacco</t>
+        </is>
+      </c>
+      <c r="F33" s="8" t="n">
+        <v>222.41</v>
+      </c>
+      <c r="G33" s="8" t="n">
+        <v>111.2</v>
+      </c>
+      <c r="J33" s="5" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="K33" s="5" t="inlineStr">
+        <is>
+          <t>Grazing Area</t>
+        </is>
+      </c>
+      <c r="L33" s="8" t="n">
+        <v>951.6</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="9" t="inlineStr">
+        <is>
+          <t>Budget</t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="n"/>
+      <c r="E34" s="5" t="inlineStr">
+        <is>
+          <t>Soyabean</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="n">
+        <v>189.79</v>
+      </c>
+      <c r="G34" s="8" t="n">
+        <v>104.38</v>
+      </c>
+      <c r="J34" s="5" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="K34" s="5" t="inlineStr">
+        <is>
           <t>Misc Area</t>
         </is>
       </c>
-      <c r="K32" s="8" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="10" t="inlineStr">
-        <is>
-          <t>Budget</t>
-        </is>
-      </c>
-      <c r="B33" s="11" t="n"/>
-      <c r="J33" s="5" t="inlineStr">
-        <is>
-          <t>Wasteland Area</t>
-        </is>
-      </c>
-      <c r="K33" s="8" t="n">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="5" t="inlineStr">
-        <is>
-          <t>Total Demand</t>
-        </is>
-      </c>
-      <c r="B34" s="9" t="n">
-        <v>3432.74</v>
-      </c>
-      <c r="J34" s="5" t="inlineStr">
-        <is>
-          <t>Fallow Area</t>
-        </is>
-      </c>
-      <c r="K34" s="8" t="n">
-        <v>2758.02</v>
+      <c r="L34" s="8" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="inlineStr">
         <is>
+          <t>Total Demand</t>
+        </is>
+      </c>
+      <c r="B35" s="11" t="n">
+        <v>23081.65</v>
+      </c>
+      <c r="E35" s="5" t="inlineStr">
+        <is>
+          <t>Masoor</t>
+        </is>
+      </c>
+      <c r="F35" s="8" t="n">
+        <v>69.69</v>
+      </c>
+      <c r="G35" s="8" t="n">
+        <v>27.88</v>
+      </c>
+      <c r="J35" s="5" t="inlineStr">
+        <is>
+          <t>Average</t>
+        </is>
+      </c>
+      <c r="K35" s="5" t="inlineStr">
+        <is>
+          <t>Wasteland Area</t>
+        </is>
+      </c>
+      <c r="L35" s="8" t="n">
+        <v>318.82</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="inlineStr">
+        <is>
           <t>Total Supply</t>
         </is>
       </c>
-      <c r="B35" s="9" t="n">
-        <v>58926.23</v>
-      </c>
-      <c r="J35" s="5" t="inlineStr">
+      <c r="B36" s="11" t="n">
+        <v>7283.73</v>
+      </c>
+      <c r="E36" s="5" t="inlineStr">
+        <is>
+          <t>Rabi pulses</t>
+        </is>
+      </c>
+      <c r="F36" s="8" t="n">
+        <v>57.45</v>
+      </c>
+      <c r="G36" s="8" t="n">
+        <v>22.98</v>
+      </c>
+      <c r="J36" s="5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="K36" s="5" t="inlineStr">
+        <is>
+          <t>Fallow Area</t>
+        </is>
+      </c>
+      <c r="L36" s="8" t="n">
+        <v>5163.64</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="5" t="inlineStr">
+        <is>
+          <t>Available Runoff</t>
+        </is>
+      </c>
+      <c r="B37" s="11" t="n">
+        <v>13755.38</v>
+      </c>
+      <c r="E37" s="5" t="inlineStr">
+        <is>
+          <t>Jowar</t>
+        </is>
+      </c>
+      <c r="F37" s="8" t="n">
+        <v>25.22</v>
+      </c>
+      <c r="G37" s="8" t="n">
+        <v>13.87</v>
+      </c>
+      <c r="J37" s="5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="K37" s="5" t="inlineStr">
         <is>
           <t>Current Fallow Area</t>
         </is>
       </c>
-      <c r="K35" s="8" t="n">
-        <v>2285</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="7" t="inlineStr">
-        <is>
-          <t>Water is Surplus in Block, No action is required.</t>
-        </is>
-      </c>
-      <c r="B36" s="12" t="n">
-        <v>55493.49000000001</v>
-      </c>
-      <c r="J36" s="5" t="inlineStr">
+      <c r="L37" s="8" t="n">
+        <v>853.92</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="5" t="inlineStr">
+        <is>
+          <t>Harvested Runoff</t>
+        </is>
+      </c>
+      <c r="B38" s="11" t="n">
+        <v>435.54</v>
+      </c>
+      <c r="E38" s="5" t="inlineStr">
+        <is>
+          <t>Gram</t>
+        </is>
+      </c>
+      <c r="F38" s="8" t="n">
+        <v>10.69</v>
+      </c>
+      <c r="G38" s="8" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="J38" s="5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="K38" s="5" t="inlineStr">
         <is>
           <t>Unirrigated Area</t>
         </is>
       </c>
-      <c r="K36" s="8" t="n">
-        <v>9375.379999999999</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="J37" s="5" t="inlineStr">
+      <c r="L38" s="8" t="n">
+        <v>18720.84</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="5" t="inlineStr">
+        <is>
+          <t>Potential Runoff</t>
+        </is>
+      </c>
+      <c r="B39" s="11" t="n">
+        <v>13319.84</v>
+      </c>
+      <c r="E39" s="5" t="inlineStr">
+        <is>
+          <t>Coriander</t>
+        </is>
+      </c>
+      <c r="F39" s="8" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="G39" s="8" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="J39" s="5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="K39" s="5" t="inlineStr">
         <is>
           <t>Canal Area</t>
         </is>
       </c>
-      <c r="K37" s="8" t="n">
-        <v>4148.46</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="J38" s="5" t="inlineStr">
+      <c r="L39" s="8" t="n">
+        <v>3845.62</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="7" t="inlineStr">
+        <is>
+          <t>Water is Deficient in Block.</t>
+        </is>
+      </c>
+      <c r="B40" s="13" t="n">
+        <v>-15797.92</v>
+      </c>
+      <c r="E40" s="5" t="inlineStr">
+        <is>
+          <t>Garlic</t>
+        </is>
+      </c>
+      <c r="F40" s="8" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="G40" s="8" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="J40" s="5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="K40" s="5" t="inlineStr">
         <is>
           <t>Tubewell Area</t>
         </is>
       </c>
-      <c r="K38" s="8" t="n">
-        <v>1164.8</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="J39" s="5" t="inlineStr">
+      <c r="L40" s="8" t="n">
+        <v>7365.56</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" s="5" t="inlineStr">
+        <is>
+          <t>Kharif pulses</t>
+        </is>
+      </c>
+      <c r="F41" s="8" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="G41" s="8" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J41" s="5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="K41" s="5" t="inlineStr">
         <is>
           <t>Tank Area</t>
         </is>
       </c>
-      <c r="K39" s="8" t="n">
-        <v>462.08</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="J40" s="5" t="inlineStr">
+      <c r="L41" s="8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" s="5" t="inlineStr">
+        <is>
+          <t>Moth</t>
+        </is>
+      </c>
+      <c r="F42" s="8" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G42" s="8" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="J42" s="5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="K42" s="5" t="inlineStr">
         <is>
           <t>Waterfall Area</t>
         </is>
       </c>
-      <c r="K40" s="8" t="n">
-        <v>148.62</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="J41" s="5" t="inlineStr">
+      <c r="L42" s="8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" s="5" t="inlineStr">
+        <is>
+          <t>Other cereals</t>
+        </is>
+      </c>
+      <c r="F43" s="8" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="G43" s="8" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="J43" s="5" t="inlineStr">
+        <is>
+          <t>Bad</t>
+        </is>
+      </c>
+      <c r="K43" s="5" t="inlineStr">
         <is>
           <t>Other Area</t>
         </is>
       </c>
-      <c r="K41" s="8" t="n">
-        <v>4315.92</v>
-      </c>
-    </row>
-    <row r="42"/>
-    <row r="43">
-      <c r="J43" s="6" t="inlineStr">
+      <c r="L43" s="8" t="n">
+        <v>123.12</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="E44" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="F44" s="10" t="n">
+        <v>39304.63</v>
+      </c>
+      <c r="G44" s="10" t="n">
+        <v>22073.65</v>
+      </c>
+      <c r="J44" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="K44" s="7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="L44" s="10" t="n">
+        <v>52924.36</v>
+      </c>
+    </row>
+    <row r="45"/>
+    <row r="46">
+      <c r="E46" s="6" t="inlineStr">
+        <is>
+          <t>d) Industry(in HaM)</t>
+        </is>
+      </c>
+      <c r="J46" s="6" t="inlineStr">
         <is>
           <t>e) Rainfall(in mm)</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="J44" s="7" t="inlineStr">
+    <row r="47">
+      <c r="E47" s="7" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="F47" s="7" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="G47" s="7" t="inlineStr">
+        <is>
+          <t>Water Allocation</t>
+        </is>
+      </c>
+      <c r="J47" s="7" t="inlineStr">
         <is>
           <t>Month-Year</t>
         </is>
       </c>
-      <c r="K44" s="7" t="inlineStr">
+      <c r="K47" s="7" t="inlineStr">
         <is>
           <t>Actual</t>
         </is>
       </c>
-      <c r="L44" s="7" t="inlineStr">
+      <c r="L47" s="7" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="J45" s="5" t="inlineStr">
+    <row r="48">
+      <c r="E48" s="5" t="inlineStr">
+        <is>
+          <t>Agriculture</t>
+        </is>
+      </c>
+      <c r="F48" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="8" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="J48" s="5" t="inlineStr">
         <is>
           <t>January-23</t>
         </is>
       </c>
-      <c r="K45" s="5" t="n">
+      <c r="K48" s="5" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="L48" s="5" t="n">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="F49" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" s="10" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="J49" s="5" t="inlineStr">
+        <is>
+          <t>February-23</t>
+        </is>
+      </c>
+      <c r="K49" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="L45" s="5" t="n">
-        <v>23.7</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="J46" s="5" t="inlineStr">
-        <is>
-          <t>February-23</t>
-        </is>
-      </c>
-      <c r="K46" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L46" s="5" t="n">
-        <v>20.8</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="J47" s="5" t="inlineStr">
-        <is>
-          <t>March-23</t>
-        </is>
-      </c>
-      <c r="K47" s="5" t="n">
-        <v>100.5</v>
-      </c>
-      <c r="L47" s="5" t="n">
-        <v>13.9</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="J48" s="5" t="inlineStr">
-        <is>
-          <t>April-23</t>
-        </is>
-      </c>
-      <c r="K48" s="5" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="L48" s="5" t="n">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="J49" s="5" t="inlineStr">
-        <is>
-          <t>May-23</t>
-        </is>
-      </c>
-      <c r="K49" s="5" t="n">
-        <v>100.6</v>
-      </c>
       <c r="L49" s="5" t="n">
-        <v>11.5</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="50">
       <c r="J50" s="5" t="inlineStr">
         <is>
-          <t>June-23</t>
+          <t>March-23</t>
         </is>
       </c>
       <c r="K50" s="5" t="n">
-        <v>95.2</v>
+        <v>21.08</v>
       </c>
       <c r="L50" s="5" t="n">
-        <v>52.7</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="51">
       <c r="J51" s="5" t="inlineStr">
         <is>
-          <t>July-23</t>
+          <t>April-23</t>
         </is>
       </c>
       <c r="K51" s="5" t="n">
-        <v>210.3</v>
+        <v>7.59</v>
       </c>
       <c r="L51" s="5" t="n">
-        <v>257.4</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="52">
       <c r="J52" s="5" t="inlineStr">
         <is>
-          <t>August-23</t>
+          <t>May-23</t>
         </is>
       </c>
       <c r="K52" s="5" t="n">
-        <v>86.8</v>
+        <v>58.22</v>
       </c>
       <c r="L52" s="5" t="n">
-        <v>257.4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53">
       <c r="J53" s="5" t="inlineStr">
         <is>
-          <t>September-23</t>
+          <t>June-23</t>
         </is>
       </c>
       <c r="K53" s="5" t="n">
-        <v>141</v>
+        <v>105.04</v>
       </c>
       <c r="L53" s="5" t="n">
-        <v>142.6</v>
+        <v>202.5</v>
       </c>
     </row>
     <row r="54">
       <c r="J54" s="5" t="inlineStr">
         <is>
-          <t>October-23</t>
+          <t>July-23</t>
         </is>
       </c>
       <c r="K54" s="5" t="n">
-        <v>57.2</v>
+        <v>142.88</v>
       </c>
       <c r="L54" s="5" t="n">
-        <v>31.2</v>
+        <v>369.4</v>
       </c>
     </row>
     <row r="55">
       <c r="J55" s="5" t="inlineStr">
         <is>
-          <t>November-23</t>
+          <t>August-23</t>
         </is>
       </c>
       <c r="K55" s="5" t="n">
-        <v>72.40000000000001</v>
+        <v>372.58</v>
       </c>
       <c r="L55" s="5" t="n">
-        <v>4.5</v>
+        <v>269.5</v>
       </c>
     </row>
     <row r="56">
       <c r="J56" s="5" t="inlineStr">
         <is>
+          <t>September-23</t>
+        </is>
+      </c>
+      <c r="K56" s="5" t="n">
+        <v>229.97</v>
+      </c>
+      <c r="L56" s="5" t="n">
+        <v>223.4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="J57" s="5" t="inlineStr">
+        <is>
+          <t>October-23</t>
+        </is>
+      </c>
+      <c r="K57" s="5" t="n">
+        <v>91.34999999999999</v>
+      </c>
+      <c r="L57" s="5" t="n">
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="J58" s="5" t="inlineStr">
+        <is>
+          <t>November-23</t>
+        </is>
+      </c>
+      <c r="K58" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" s="5" t="n">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="J59" s="5" t="inlineStr">
+        <is>
           <t>December-23</t>
         </is>
       </c>
-      <c r="K56" s="5" t="n">
-        <v>124.4</v>
-      </c>
-      <c r="L56" s="5" t="n">
-        <v>9.9</v>
+      <c r="K59" s="5" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="L59" s="5" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="J60" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="K60" s="7" t="n">
+        <v>1032.08</v>
+      </c>
+      <c r="L60" s="7" t="n">
+        <v>1294.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J14:L14"/>
     <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="J28:L28"/>
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="J46:L46"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J20:L20"/>
     <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="E21:G21"/>
     <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor runoff calculations and update Excel export functionality
</commit_message>
<xml_diff>
--- a/iJal/app/static/assets/water_budget.xlsx
+++ b/iJal/app/static/assets/water_budget.xlsx
@@ -1040,7 +1040,7 @@
       </c>
       <c r="K22" s="7" t="inlineStr">
         <is>
-          <t>% Runoff</t>
+          <t>Area</t>
         </is>
       </c>
       <c r="L22" s="7" t="inlineStr">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="K23" s="8" t="n">
-        <v>38.6</v>
+        <v>15427.24</v>
       </c>
       <c r="L23" s="8" t="n">
         <v>3983.83</v>
@@ -1109,7 +1109,7 @@
         </is>
       </c>
       <c r="K24" s="8" t="n">
-        <v>28.9</v>
+        <v>1416.42</v>
       </c>
       <c r="L24" s="8" t="n">
         <v>2982.71</v>
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="K25" s="8" t="n">
-        <v>19.3</v>
+        <v>36080.7</v>
       </c>
       <c r="L25" s="8" t="n">
         <v>1991.91</v>
@@ -1176,7 +1176,9 @@
           <t>Total</t>
         </is>
       </c>
-      <c r="K26" s="7" t="inlineStr"/>
+      <c r="K26" s="10" t="n">
+        <v>52924.36</v>
+      </c>
       <c r="L26" s="10" t="n">
         <v>8958.450000000001</v>
       </c>

</xml_diff>